<commit_message>
add generate footer form, and fill all tbl on form
</commit_message>
<xml_diff>
--- a/reportOP8.xlsx
+++ b/reportOP8.xlsx
@@ -70,7 +70,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
@@ -99,6 +99,9 @@
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -397,7 +400,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BY31"/>
+  <dimension ref="A1:BY82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -550,12 +553,12 @@
     <row r="8">
       <c r="A8" s="4" t="inlineStr">
         <is>
-          <t>Преподавательская</t>
+          <t>Кафе уют</t>
         </is>
       </c>
       <c r="BQ8" s="2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -579,7 +582,7 @@
       </c>
       <c r="BQ10" s="2" t="inlineStr">
         <is>
-          <t>1488</t>
+          <t>228</t>
         </is>
       </c>
     </row>
@@ -627,7 +630,7 @@
       </c>
       <c r="BM13" s="7" t="inlineStr">
         <is>
-          <t>Вор в законе</t>
+          <t>БОСС</t>
         </is>
       </c>
     </row>
@@ -639,22 +642,22 @@
       </c>
       <c r="AK14" s="6" t="inlineStr">
         <is>
-          <t>1488</t>
+          <t>1337</t>
         </is>
       </c>
       <c r="AS14" s="6" t="inlineStr">
         <is>
-          <t>11.11.1768</t>
+          <t>15.05.2018</t>
         </is>
       </c>
       <c r="BA14" s="6" t="inlineStr">
         <is>
-          <t>23.04.5232</t>
+          <t>01.03.2018</t>
         </is>
       </c>
       <c r="BF14" s="6" t="inlineStr">
         <is>
-          <t>23.04.3124</t>
+          <t>27.03.2018</t>
         </is>
       </c>
       <c r="BM14" s="9" t="inlineStr">
@@ -666,7 +669,7 @@
     <row r="15">
       <c r="BQ15" s="9" t="inlineStr">
         <is>
-          <t>Зыбенко Михаил петрович</t>
+          <t>Зыбенко Михали Петрович</t>
         </is>
       </c>
     </row>
@@ -695,7 +698,7 @@
       </c>
       <c r="BL17" s="12" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>12</t>
         </is>
       </c>
       <c r="BM17" s="11" t="inlineStr">
@@ -705,12 +708,12 @@
       </c>
       <c r="BN17" s="12" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>05</t>
         </is>
       </c>
       <c r="BV17" s="12" t="inlineStr">
         <is>
-          <t>3412</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="BX17" s="2" t="inlineStr">
@@ -732,7 +735,7 @@
       </c>
       <c r="AM18" s="4" t="inlineStr">
         <is>
-          <t>Карлов Геннадий Петрович</t>
+          <t>Кривосок Геннадий Михайлович</t>
         </is>
       </c>
     </row>
@@ -873,7 +876,7 @@
       </c>
       <c r="E27" s="2" t="inlineStr">
         <is>
-          <t>стакан</t>
+          <t>2</t>
         </is>
       </c>
       <c r="O27" s="2" t="inlineStr">
@@ -883,133 +886,131 @@
       </c>
       <c r="T27" s="2" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>4</t>
         </is>
       </c>
       <c r="Z27" s="2" t="inlineStr">
         <is>
-          <t>124</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AD27" s="2" t="inlineStr">
         <is>
-          <t>4216</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AI27" s="2" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>7</t>
         </is>
       </c>
       <c r="AM27" s="2" t="inlineStr">
         <is>
-          <t>1428</t>
+          <t>8</t>
         </is>
       </c>
       <c r="AR27" s="2" t="inlineStr">
         <is>
-          <t>166</t>
+          <t>9</t>
         </is>
       </c>
       <c r="AV27" s="2" t="inlineStr">
         <is>
-          <t>5644</t>
+          <t>10</t>
         </is>
       </c>
       <c r="BA27" s="2" t="inlineStr">
         <is>
-          <t>как хрустальные
-кудал то делось</t>
+          <t>11</t>
         </is>
       </c>
       <c r="BR27" s="2" t="inlineStr">
         <is>
-          <t>сижу не пержу</t>
+          <t>12</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E28" s="2" t="inlineStr">
         <is>
-          <t>вилка</t>
+          <t>ложка</t>
         </is>
       </c>
       <c r="O28" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="T28" s="2" t="inlineStr">
         <is>
-          <t>736</t>
+          <t>100</t>
         </is>
       </c>
       <c r="Z28" s="2" t="inlineStr">
         <is>
-          <t>7254</t>
+          <t>20</t>
         </is>
       </c>
       <c r="AD28" s="2" t="inlineStr">
         <is>
-          <t>5338944</t>
+          <t>2000</t>
         </is>
       </c>
       <c r="AI28" s="2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AM28" s="2" t="inlineStr">
         <is>
-          <t>3680</t>
+          <t>400</t>
         </is>
       </c>
       <c r="AR28" s="2" t="inlineStr">
         <is>
-          <t>7259</t>
+          <t>24</t>
         </is>
       </c>
       <c r="AV28" s="2" t="inlineStr">
         <is>
-          <t>5342624</t>
+          <t>2400</t>
         </is>
       </c>
       <c r="BA28" s="2" t="inlineStr">
         <is>
-          <t>в глаз?
-хз что произошло</t>
+          <t>Проверяли как гнется, Кидались в другую компанию</t>
         </is>
       </c>
       <c r="BR28" s="2" t="inlineStr">
         <is>
-          <t>лабы пилю</t>
+          <t>топ ложка</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E29" s="2" t="inlineStr">
         <is>
-          <t>кружка</t>
+          <t>вилка</t>
         </is>
       </c>
       <c r="O29" s="2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="T29" s="2" t="inlineStr">
         <is>
-          <t>9256</t>
+          <t>40</t>
         </is>
       </c>
       <c r="Z29" s="2" t="inlineStr">
@@ -1044,144 +1045,1016 @@
       </c>
       <c r="BA29" s="2" t="inlineStr">
         <is>
-          <t>все нормас
-ничего не было</t>
+          <t>Забыли где они вообще лежат, Не использовали</t>
         </is>
       </c>
       <c r="BR29" s="2" t="inlineStr">
         <is>
-          <t>ето круженция</t>
+          <t>норм вилка</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="inlineStr">
         <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="inlineStr">
+        <is>
+          <t>кружка</t>
+        </is>
+      </c>
+      <c r="O30" s="2" t="inlineStr">
+        <is>
           <t>4</t>
         </is>
       </c>
-      <c r="E30" s="2" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="O30" s="2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="T30" s="2" t="inlineStr">
         <is>
-          <t>523</t>
+          <t>99</t>
         </is>
       </c>
       <c r="Z30" s="2" t="inlineStr">
         <is>
-          <t>244</t>
+          <t>65</t>
         </is>
       </c>
       <c r="AD30" s="2" t="inlineStr">
         <is>
-          <t>127612</t>
+          <t>6435</t>
         </is>
       </c>
       <c r="AI30" s="2" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>12</t>
         </is>
       </c>
       <c r="AM30" s="2" t="inlineStr">
         <is>
-          <t>22489</t>
+          <t>1188</t>
         </is>
       </c>
       <c r="AR30" s="2" t="inlineStr">
         <is>
-          <t>287</t>
+          <t>77</t>
         </is>
       </c>
       <c r="AV30" s="2" t="inlineStr">
         <is>
-          <t>150101</t>
+          <t>7623</t>
         </is>
       </c>
       <c r="BA30" s="2" t="inlineStr">
         <is>
-          <t>до сих пор не известно
-это хз что</t>
+          <t>Катали их много, Играли ими в гольф</t>
         </is>
       </c>
       <c r="BR30" s="2" t="inlineStr">
         <is>
-          <t>это из тех что не определилась</t>
+          <t>хорошая круженция</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="inlineStr">
+        <is>
+          <t>стакан</t>
+        </is>
+      </c>
+      <c r="O31" s="2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="T31" s="2" t="inlineStr">
+        <is>
+          <t>4000</t>
+        </is>
+      </c>
+      <c r="Z31" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AD31" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AI31" s="2" t="inlineStr">
+        <is>
+          <t>89</t>
+        </is>
+      </c>
+      <c r="AM31" s="2" t="inlineStr">
+        <is>
+          <t>356000</t>
+        </is>
+      </c>
+      <c r="AR31" s="2" t="inlineStr">
+        <is>
+          <t>89</t>
+        </is>
+      </c>
+      <c r="AV31" s="2" t="inlineStr">
+        <is>
+          <t>356000</t>
+        </is>
+      </c>
+      <c r="BA31" s="2" t="inlineStr">
+        <is>
+          <t>Взрывы молекул, Кидали в окна</t>
+        </is>
+      </c>
+      <c r="BR31" s="2" t="inlineStr">
+        <is>
+          <t>балдежный стакан</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="inlineStr">
+        <is>
           <t>5</t>
         </is>
       </c>
-      <c r="E31" s="2" t="inlineStr">
+      <c r="E32" s="2" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O32" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T32" s="2" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="Z32" s="2" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="AD32" s="2" t="inlineStr">
+        <is>
+          <t>960</t>
+        </is>
+      </c>
+      <c r="AI32" s="2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AM32" s="2" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="AR32" s="2" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="AV32" s="2" t="inlineStr">
+        <is>
+          <t>1020</t>
+        </is>
+      </c>
+      <c r="BA32" s="2" t="inlineStr">
+        <is>
+          <t>Надо для начала понять что это, Повариха утащила</t>
+        </is>
+      </c>
+      <c r="BR32" s="2" t="inlineStr">
+        <is>
+          <t>забыл что за тип</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="inlineStr">
+        <is>
+          <t>тарелка</t>
+        </is>
+      </c>
+      <c r="O33" s="2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="T33" s="2" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="Z33" s="2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="AD33" s="2" t="inlineStr">
+        <is>
+          <t>224</t>
+        </is>
+      </c>
+      <c r="AI33" s="2" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="AM33" s="2" t="inlineStr">
+        <is>
+          <t>3360</t>
+        </is>
+      </c>
+      <c r="AR33" s="2" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="AV33" s="2" t="inlineStr">
+        <is>
+          <t>3584</t>
+        </is>
+      </c>
+      <c r="BA33" s="2" t="inlineStr">
+        <is>
+          <t>Игра в фрисби не прощает тарелок, Улетела при игре в фрисби</t>
+        </is>
+      </c>
+      <c r="BR33" s="2" t="inlineStr">
+        <is>
+          <t>тарелка круглая</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="inlineStr">
         <is>
           <t>ложка</t>
         </is>
       </c>
-      <c r="O31" s="2" t="inlineStr">
+      <c r="O34" s="2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="T31" s="2" t="inlineStr">
-        <is>
-          <t>742</t>
-        </is>
-      </c>
-      <c r="Z31" s="2" t="inlineStr">
-        <is>
-          <t>789</t>
-        </is>
-      </c>
-      <c r="AD31" s="2" t="inlineStr">
-        <is>
-          <t>585438</t>
-        </is>
-      </c>
-      <c r="AI31" s="2" t="inlineStr">
-        <is>
-          <t>78</t>
-        </is>
-      </c>
-      <c r="AM31" s="2" t="inlineStr">
-        <is>
-          <t>57876</t>
-        </is>
-      </c>
-      <c r="AR31" s="2" t="inlineStr">
-        <is>
-          <t>867</t>
-        </is>
-      </c>
-      <c r="AV31" s="2" t="inlineStr">
-        <is>
-          <t>643314</t>
-        </is>
-      </c>
-      <c r="BA31" s="2" t="inlineStr">
-        <is>
-          <t>ложкой раз
-мда мда</t>
-        </is>
-      </c>
-      <c r="BR31" s="2" t="inlineStr">
-        <is>
-          <t>ложечка</t>
-        </is>
-      </c>
-    </row>
+      <c r="T34" s="2" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="Z34" s="2" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+      <c r="AD34" s="2" t="inlineStr">
+        <is>
+          <t>4560</t>
+        </is>
+      </c>
+      <c r="AI34" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AM34" s="2" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="AR34" s="2" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
+      </c>
+      <c r="AV34" s="2" t="inlineStr">
+        <is>
+          <t>4640</t>
+        </is>
+      </c>
+      <c r="BA34" s="2" t="inlineStr">
+        <is>
+          <t>Ложки легко гнутся, Утанула в еде</t>
+        </is>
+      </c>
+      <c r="BR34" s="2" t="inlineStr">
+        <is>
+          <t>ложка целая</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="inlineStr"/>
+      <c r="E35" s="2" t="inlineStr"/>
+      <c r="O35" s="2" t="inlineStr"/>
+      <c r="T35" s="2" t="inlineStr"/>
+      <c r="Z35" s="2" t="inlineStr"/>
+      <c r="AD35" s="2" t="inlineStr"/>
+      <c r="AI35" s="2" t="inlineStr"/>
+      <c r="AM35" s="2" t="inlineStr"/>
+      <c r="AR35" s="2" t="inlineStr"/>
+      <c r="AV35" s="2" t="inlineStr"/>
+      <c r="BA35" s="2" t="inlineStr"/>
+      <c r="BR35" s="2" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="inlineStr"/>
+      <c r="E36" s="2" t="inlineStr"/>
+      <c r="O36" s="2" t="inlineStr"/>
+      <c r="T36" s="2" t="inlineStr"/>
+      <c r="Z36" s="2" t="inlineStr"/>
+      <c r="AD36" s="2" t="inlineStr"/>
+      <c r="AI36" s="2" t="inlineStr"/>
+      <c r="AM36" s="2" t="inlineStr"/>
+      <c r="AR36" s="2" t="inlineStr"/>
+      <c r="AV36" s="2" t="inlineStr"/>
+      <c r="BA36" s="2" t="inlineStr"/>
+      <c r="BR36" s="2" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="inlineStr"/>
+      <c r="E37" s="2" t="inlineStr"/>
+      <c r="O37" s="2" t="inlineStr"/>
+      <c r="T37" s="2" t="inlineStr"/>
+      <c r="Z37" s="2" t="inlineStr"/>
+      <c r="AD37" s="2" t="inlineStr"/>
+      <c r="AI37" s="2" t="inlineStr"/>
+      <c r="AM37" s="2" t="inlineStr"/>
+      <c r="AR37" s="2" t="inlineStr"/>
+      <c r="AV37" s="2" t="inlineStr"/>
+      <c r="BA37" s="2" t="inlineStr"/>
+      <c r="BR37" s="2" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="inlineStr"/>
+      <c r="E38" s="2" t="inlineStr"/>
+      <c r="O38" s="2" t="inlineStr"/>
+      <c r="T38" s="2" t="inlineStr">
+        <is>
+          <t>Итого</t>
+        </is>
+      </c>
+      <c r="Z38" s="2" t="inlineStr">
+        <is>
+          <t>194</t>
+        </is>
+      </c>
+      <c r="AD38" s="2" t="inlineStr">
+        <is>
+          <t>14179</t>
+        </is>
+      </c>
+      <c r="AI38" s="2" t="inlineStr">
+        <is>
+          <t>169</t>
+        </is>
+      </c>
+      <c r="AM38" s="2" t="inlineStr">
+        <is>
+          <t>361088</t>
+        </is>
+      </c>
+      <c r="AR38" s="2" t="inlineStr">
+        <is>
+          <t>363</t>
+        </is>
+      </c>
+      <c r="AV38" s="2" t="inlineStr">
+        <is>
+          <t>375267</t>
+        </is>
+      </c>
+      <c r="BA38" s="2" t="inlineStr"/>
+      <c r="BR38" s="2" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="BE39" s="4" t="inlineStr">
+        <is>
+          <t>Оборотная сторона формы № ОП-8</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="inlineStr">
+        <is>
+          <t>Но-
+мер
+по по-
+рядку</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="inlineStr">
+        <is>
+          <t>Посуда, приборы</t>
+        </is>
+      </c>
+      <c r="T41" s="2" t="inlineStr">
+        <is>
+          <t>Цена,
+руб. коп.</t>
+        </is>
+      </c>
+      <c r="Z41" s="2" t="inlineStr">
+        <is>
+          <t>Бой, лом, утрачено, пропало</t>
+        </is>
+      </c>
+      <c r="BA41" s="2" t="inlineStr">
+        <is>
+          <t>Обстоятельства
+боя, лома, утраты, пропажи.
+Виновные лица
+(должность, фамилия, и., о.)</t>
+        </is>
+      </c>
+      <c r="BR41" s="2" t="inlineStr">
+        <is>
+          <t>Примечание</t>
+        </is>
+      </c>
+    </row>
+    <row r="42"/>
+    <row r="43">
+      <c r="E43" s="2" t="inlineStr">
+        <is>
+          <t>наименование</t>
+        </is>
+      </c>
+      <c r="O43" s="2" t="inlineStr">
+        <is>
+          <t>код</t>
+        </is>
+      </c>
+      <c r="Z43" s="2" t="inlineStr">
+        <is>
+          <t>бой, лом </t>
+        </is>
+      </c>
+      <c r="AI43" s="2" t="inlineStr">
+        <is>
+          <t>утрачено, пропало</t>
+        </is>
+      </c>
+      <c r="AR43" s="2" t="inlineStr">
+        <is>
+          <t>всего</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="Z44" s="2" t="inlineStr">
+        <is>
+          <t>коли-
+чество,
+шт.</t>
+        </is>
+      </c>
+      <c r="AD44" s="2" t="inlineStr">
+        <is>
+          <t>сумма,
+руб. коп.</t>
+        </is>
+      </c>
+      <c r="AI44" s="2" t="inlineStr">
+        <is>
+          <t>коли-
+чество,
+шт.</t>
+        </is>
+      </c>
+      <c r="AM44" s="2" t="inlineStr">
+        <is>
+          <t>сумма,
+руб. коп.</t>
+        </is>
+      </c>
+      <c r="AR44" s="2" t="inlineStr">
+        <is>
+          <t>коли-
+чество,
+шт.</t>
+        </is>
+      </c>
+      <c r="AV44" s="2" t="inlineStr">
+        <is>
+          <t>сумма,
+руб. коп.</t>
+        </is>
+      </c>
+    </row>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47">
+      <c r="A47" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E47" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O47" s="2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="T47" s="2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="Z47" s="2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AD47" s="2" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="AI47" s="2" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="AM47" s="2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="AR47" s="2" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="AV47" s="2" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="BA47" s="2" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="BR47" s="2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="inlineStr"/>
+      <c r="E48" s="2" t="inlineStr"/>
+      <c r="O48" s="2" t="inlineStr"/>
+      <c r="T48" s="2" t="inlineStr"/>
+      <c r="Z48" s="2" t="inlineStr"/>
+      <c r="AD48" s="2" t="inlineStr"/>
+      <c r="AI48" s="2" t="inlineStr"/>
+      <c r="AM48" s="2" t="inlineStr"/>
+      <c r="AR48" s="2" t="inlineStr"/>
+      <c r="AV48" s="2" t="inlineStr"/>
+      <c r="BA48" s="2" t="inlineStr"/>
+      <c r="BR48" s="2" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="inlineStr"/>
+      <c r="E49" s="2" t="inlineStr"/>
+      <c r="O49" s="2" t="inlineStr"/>
+      <c r="T49" s="2" t="inlineStr"/>
+      <c r="Z49" s="2" t="inlineStr"/>
+      <c r="AD49" s="2" t="inlineStr"/>
+      <c r="AI49" s="2" t="inlineStr"/>
+      <c r="AM49" s="2" t="inlineStr"/>
+      <c r="AR49" s="2" t="inlineStr"/>
+      <c r="AV49" s="2" t="inlineStr"/>
+      <c r="BA49" s="2" t="inlineStr"/>
+      <c r="BR49" s="2" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="inlineStr"/>
+      <c r="E50" s="2" t="inlineStr"/>
+      <c r="O50" s="2" t="inlineStr"/>
+      <c r="T50" s="2" t="inlineStr"/>
+      <c r="Z50" s="2" t="inlineStr"/>
+      <c r="AD50" s="2" t="inlineStr"/>
+      <c r="AI50" s="2" t="inlineStr"/>
+      <c r="AM50" s="2" t="inlineStr"/>
+      <c r="AR50" s="2" t="inlineStr"/>
+      <c r="AV50" s="2" t="inlineStr"/>
+      <c r="BA50" s="2" t="inlineStr"/>
+      <c r="BR50" s="2" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="inlineStr"/>
+      <c r="E51" s="2" t="inlineStr"/>
+      <c r="O51" s="2" t="inlineStr"/>
+      <c r="T51" s="2" t="inlineStr"/>
+      <c r="Z51" s="2" t="inlineStr"/>
+      <c r="AD51" s="2" t="inlineStr"/>
+      <c r="AI51" s="2" t="inlineStr"/>
+      <c r="AM51" s="2" t="inlineStr"/>
+      <c r="AR51" s="2" t="inlineStr"/>
+      <c r="AV51" s="2" t="inlineStr"/>
+      <c r="BA51" s="2" t="inlineStr"/>
+      <c r="BR51" s="2" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="inlineStr"/>
+      <c r="E52" s="2" t="inlineStr"/>
+      <c r="O52" s="2" t="inlineStr"/>
+      <c r="T52" s="2" t="inlineStr"/>
+      <c r="Z52" s="2" t="inlineStr"/>
+      <c r="AD52" s="2" t="inlineStr"/>
+      <c r="AI52" s="2" t="inlineStr"/>
+      <c r="AM52" s="2" t="inlineStr"/>
+      <c r="AR52" s="2" t="inlineStr"/>
+      <c r="AV52" s="2" t="inlineStr"/>
+      <c r="BA52" s="2" t="inlineStr"/>
+      <c r="BR52" s="2" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="inlineStr"/>
+      <c r="E53" s="2" t="inlineStr"/>
+      <c r="O53" s="2" t="inlineStr"/>
+      <c r="T53" s="2" t="inlineStr"/>
+      <c r="Z53" s="2" t="inlineStr"/>
+      <c r="AD53" s="2" t="inlineStr"/>
+      <c r="AI53" s="2" t="inlineStr"/>
+      <c r="AM53" s="2" t="inlineStr"/>
+      <c r="AR53" s="2" t="inlineStr"/>
+      <c r="AV53" s="2" t="inlineStr"/>
+      <c r="BA53" s="2" t="inlineStr"/>
+      <c r="BR53" s="2" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="inlineStr"/>
+      <c r="E54" s="2" t="inlineStr"/>
+      <c r="O54" s="2" t="inlineStr"/>
+      <c r="T54" s="2" t="inlineStr"/>
+      <c r="Z54" s="2" t="inlineStr"/>
+      <c r="AD54" s="2" t="inlineStr"/>
+      <c r="AI54" s="2" t="inlineStr"/>
+      <c r="AM54" s="2" t="inlineStr"/>
+      <c r="AR54" s="2" t="inlineStr"/>
+      <c r="AV54" s="2" t="inlineStr"/>
+      <c r="BA54" s="2" t="inlineStr"/>
+      <c r="BR54" s="2" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="inlineStr"/>
+      <c r="E55" s="2" t="inlineStr"/>
+      <c r="O55" s="2" t="inlineStr"/>
+      <c r="T55" s="2" t="inlineStr"/>
+      <c r="Z55" s="2" t="inlineStr"/>
+      <c r="AD55" s="2" t="inlineStr"/>
+      <c r="AI55" s="2" t="inlineStr"/>
+      <c r="AM55" s="2" t="inlineStr"/>
+      <c r="AR55" s="2" t="inlineStr"/>
+      <c r="AV55" s="2" t="inlineStr"/>
+      <c r="BA55" s="2" t="inlineStr"/>
+      <c r="BR55" s="2" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="inlineStr"/>
+      <c r="E56" s="2" t="inlineStr"/>
+      <c r="O56" s="2" t="inlineStr"/>
+      <c r="T56" s="2" t="inlineStr"/>
+      <c r="Z56" s="2" t="inlineStr"/>
+      <c r="AD56" s="2" t="inlineStr"/>
+      <c r="AI56" s="2" t="inlineStr"/>
+      <c r="AM56" s="2" t="inlineStr"/>
+      <c r="AR56" s="2" t="inlineStr"/>
+      <c r="AV56" s="2" t="inlineStr"/>
+      <c r="BA56" s="2" t="inlineStr"/>
+      <c r="BR56" s="2" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="inlineStr"/>
+      <c r="E57" s="2" t="inlineStr"/>
+      <c r="O57" s="2" t="inlineStr"/>
+      <c r="T57" s="2" t="inlineStr"/>
+      <c r="Z57" s="2" t="inlineStr"/>
+      <c r="AD57" s="2" t="inlineStr"/>
+      <c r="AI57" s="2" t="inlineStr"/>
+      <c r="AM57" s="2" t="inlineStr"/>
+      <c r="AR57" s="2" t="inlineStr"/>
+      <c r="AV57" s="2" t="inlineStr"/>
+      <c r="BA57" s="2" t="inlineStr"/>
+      <c r="BR57" s="2" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="inlineStr"/>
+      <c r="E58" s="2" t="inlineStr"/>
+      <c r="O58" s="2" t="inlineStr"/>
+      <c r="T58" s="2" t="inlineStr">
+        <is>
+          <t>Итого</t>
+        </is>
+      </c>
+      <c r="Z58" s="2" t="inlineStr"/>
+      <c r="AD58" s="2" t="inlineStr"/>
+      <c r="AI58" s="2" t="inlineStr"/>
+      <c r="AM58" s="2" t="inlineStr"/>
+      <c r="AR58" s="2" t="inlineStr"/>
+      <c r="AV58" s="2" t="inlineStr"/>
+      <c r="BA58" s="2" t="inlineStr"/>
+      <c r="BR58" s="2" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="inlineStr"/>
+      <c r="E59" s="2" t="inlineStr"/>
+      <c r="O59" s="2" t="inlineStr"/>
+      <c r="T59" s="2" t="inlineStr">
+        <is>
+          <t>Всего</t>
+        </is>
+      </c>
+      <c r="Z59" s="2" t="inlineStr">
+        <is>
+          <t>194</t>
+        </is>
+      </c>
+      <c r="AD59" s="2" t="inlineStr">
+        <is>
+          <t>14179</t>
+        </is>
+      </c>
+      <c r="AI59" s="2" t="inlineStr">
+        <is>
+          <t>169</t>
+        </is>
+      </c>
+      <c r="AM59" s="2" t="inlineStr">
+        <is>
+          <t>361088</t>
+        </is>
+      </c>
+      <c r="AR59" s="2" t="inlineStr">
+        <is>
+          <t>363</t>
+        </is>
+      </c>
+      <c r="AV59" s="2" t="inlineStr">
+        <is>
+          <t>375267</t>
+        </is>
+      </c>
+      <c r="BA59" s="2" t="inlineStr"/>
+      <c r="BR59" s="2" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="3" t="inlineStr">
+        <is>
+          <t>Перечисленные в графе «Бой, лом» столовая посуда и приборы в количестве</t>
+        </is>
+      </c>
+      <c r="AI60" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BG60" s="3" t="inlineStr">
+        <is>
+          <t>шт. уничтожены в нашем присутствии</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="AI61" s="2" t="inlineStr">
+        <is>
+          <t>(печатно)</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="E63" s="2" t="inlineStr">
+        <is>
+          <t>Члены комиссии:</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="N64" s="2" t="inlineStr">
+        <is>
+          <t>Заведующий</t>
+        </is>
+      </c>
+      <c r="AQ64" s="2" t="inlineStr">
+        <is>
+          <t>Лебедев Алексей Андреевич</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="N65" s="7" t="inlineStr">
+        <is>
+          <t>(должность)</t>
+        </is>
+      </c>
+      <c r="AD65" s="7" t="inlineStr">
+        <is>
+          <t>(подпись)</t>
+        </is>
+      </c>
+      <c r="AQ65" s="7" t="inlineStr">
+        <is>
+          <t>(расшифровка подписи)</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="N66" s="2" t="inlineStr">
+        <is>
+          <t>Глава 1</t>
+        </is>
+      </c>
+      <c r="AQ66" s="2" t="inlineStr">
+        <is>
+          <t>Кол Владимир Алексеевич</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="N67" s="7" t="inlineStr">
+        <is>
+          <t>(должность)</t>
+        </is>
+      </c>
+      <c r="AD67" s="7" t="inlineStr">
+        <is>
+          <t>(подпись)</t>
+        </is>
+      </c>
+      <c r="AQ67" s="7" t="inlineStr">
+        <is>
+          <t>(расшифровка подписи)</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="N68" s="2" t="inlineStr">
+        <is>
+          <t>Глава 2</t>
+        </is>
+      </c>
+      <c r="AQ68" s="2" t="inlineStr">
+        <is>
+          <t>Лиловая Ольга Васильевна</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="N69" s="7" t="inlineStr">
+        <is>
+          <t>(должность)</t>
+        </is>
+      </c>
+      <c r="AD69" s="7" t="inlineStr">
+        <is>
+          <t>(подпись)</t>
+        </is>
+      </c>
+      <c r="AQ69" s="7" t="inlineStr">
+        <is>
+          <t>(расшифровка подписи)</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="N70" s="2" t="inlineStr">
+        <is>
+          <t>Зам главы</t>
+        </is>
+      </c>
+      <c r="AQ70" s="2" t="inlineStr">
+        <is>
+          <t>Кавровая Александра Валерьевна</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="N71" s="7" t="inlineStr">
+        <is>
+          <t>(должность)</t>
+        </is>
+      </c>
+      <c r="AD71" s="7" t="inlineStr">
+        <is>
+          <t>(подпись)</t>
+        </is>
+      </c>
+      <c r="AQ71" s="7" t="inlineStr">
+        <is>
+          <t>(расшифровка подписи)</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="N72" s="2" t="inlineStr">
+        <is>
+          <t>Главный охранник</t>
+        </is>
+      </c>
+      <c r="AQ72" s="2" t="inlineStr">
+        <is>
+          <t>Красноухов Виталий Дмитриевич</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="N73" s="7" t="inlineStr">
+        <is>
+          <t>(должность)</t>
+        </is>
+      </c>
+      <c r="AD73" s="7" t="inlineStr">
+        <is>
+          <t>(подпись)</t>
+        </is>
+      </c>
+      <c r="AQ73" s="7" t="inlineStr">
+        <is>
+          <t>(расшифровка подписи)</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="N74" s="2" t="inlineStr">
+        <is>
+          <t>Зам охранника</t>
+        </is>
+      </c>
+      <c r="AQ74" s="2" t="inlineStr">
+        <is>
+          <t>Сыромолот Анастасия Викторовна</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="N75" s="7" t="inlineStr">
+        <is>
+          <t>(должность)</t>
+        </is>
+      </c>
+      <c r="AD75" s="7" t="inlineStr">
+        <is>
+          <t>(подпись)</t>
+        </is>
+      </c>
+      <c r="AQ75" s="7" t="inlineStr">
+        <is>
+          <t>(расшифровка подписи)</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="3" t="inlineStr">
+        <is>
+          <t>Решение администрации:</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="13" t="inlineStr">
+        <is>
+          <t>Все плохо, все поломали, немного сохранили, ууууу да кто так работает это просто невозможно, надо всех пувольнять, а если нет, то выговоры всем уууу
+Да серьезно столько всего испортили за такой промежуток времени это сложно терпеть. Так завтра что выговоры писал все уууууууууууууууууууууууууууууууу
+ууууууууууууууууууууууууууууу
+уууууууууууууууууу</t>
+        </is>
+      </c>
+    </row>
+    <row r="79"/>
+    <row r="80"/>
+    <row r="81"/>
+    <row r="82"/>
   </sheetData>
-  <mergeCells count="110">
+  <mergeCells count="407">
     <mergeCell ref="BQ4:BX4"/>
     <mergeCell ref="BQ5:BX5"/>
     <mergeCell ref="BQ6:BX6"/>
@@ -1292,6 +2165,303 @@
     <mergeCell ref="AV31:AZ31"/>
     <mergeCell ref="BA31:BQ31"/>
     <mergeCell ref="BR31:BX31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="E32:N32"/>
+    <mergeCell ref="O32:S32"/>
+    <mergeCell ref="T32:Y32"/>
+    <mergeCell ref="Z32:AC32"/>
+    <mergeCell ref="AD32:AH32"/>
+    <mergeCell ref="AI32:AL32"/>
+    <mergeCell ref="AM32:AQ32"/>
+    <mergeCell ref="AR32:AU32"/>
+    <mergeCell ref="AV32:AZ32"/>
+    <mergeCell ref="BA32:BQ32"/>
+    <mergeCell ref="BR32:BX32"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="E33:N33"/>
+    <mergeCell ref="O33:S33"/>
+    <mergeCell ref="T33:Y33"/>
+    <mergeCell ref="Z33:AC33"/>
+    <mergeCell ref="AD33:AH33"/>
+    <mergeCell ref="AI33:AL33"/>
+    <mergeCell ref="AM33:AQ33"/>
+    <mergeCell ref="AR33:AU33"/>
+    <mergeCell ref="AV33:AZ33"/>
+    <mergeCell ref="BA33:BQ33"/>
+    <mergeCell ref="BR33:BX33"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="E34:N34"/>
+    <mergeCell ref="O34:S34"/>
+    <mergeCell ref="T34:Y34"/>
+    <mergeCell ref="Z34:AC34"/>
+    <mergeCell ref="AD34:AH34"/>
+    <mergeCell ref="AI34:AL34"/>
+    <mergeCell ref="AM34:AQ34"/>
+    <mergeCell ref="AR34:AU34"/>
+    <mergeCell ref="AV34:AZ34"/>
+    <mergeCell ref="BA34:BQ34"/>
+    <mergeCell ref="BR34:BX34"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="E35:N35"/>
+    <mergeCell ref="O35:S35"/>
+    <mergeCell ref="T35:Y35"/>
+    <mergeCell ref="Z35:AC35"/>
+    <mergeCell ref="AD35:AH35"/>
+    <mergeCell ref="AI35:AL35"/>
+    <mergeCell ref="AM35:AQ35"/>
+    <mergeCell ref="AR35:AU35"/>
+    <mergeCell ref="AV35:AZ35"/>
+    <mergeCell ref="BA35:BQ35"/>
+    <mergeCell ref="BR35:BX35"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="E36:N36"/>
+    <mergeCell ref="O36:S36"/>
+    <mergeCell ref="T36:Y36"/>
+    <mergeCell ref="Z36:AC36"/>
+    <mergeCell ref="AD36:AH36"/>
+    <mergeCell ref="AI36:AL36"/>
+    <mergeCell ref="AM36:AQ36"/>
+    <mergeCell ref="AR36:AU36"/>
+    <mergeCell ref="AV36:AZ36"/>
+    <mergeCell ref="BA36:BQ36"/>
+    <mergeCell ref="BR36:BX36"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="E37:N37"/>
+    <mergeCell ref="O37:S37"/>
+    <mergeCell ref="T37:Y37"/>
+    <mergeCell ref="Z37:AC37"/>
+    <mergeCell ref="AD37:AH37"/>
+    <mergeCell ref="AI37:AL37"/>
+    <mergeCell ref="AM37:AQ37"/>
+    <mergeCell ref="AR37:AU37"/>
+    <mergeCell ref="AV37:AZ37"/>
+    <mergeCell ref="BA37:BQ37"/>
+    <mergeCell ref="BR37:BX37"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="E38:N38"/>
+    <mergeCell ref="O38:S38"/>
+    <mergeCell ref="T38:Y38"/>
+    <mergeCell ref="Z38:AC38"/>
+    <mergeCell ref="AD38:AH38"/>
+    <mergeCell ref="AI38:AL38"/>
+    <mergeCell ref="AM38:AQ38"/>
+    <mergeCell ref="AR38:AU38"/>
+    <mergeCell ref="AV38:AZ38"/>
+    <mergeCell ref="BA38:BQ38"/>
+    <mergeCell ref="BR38:BX38"/>
+    <mergeCell ref="BE39:BX39"/>
+    <mergeCell ref="A41:D46"/>
+    <mergeCell ref="E41:S42"/>
+    <mergeCell ref="E43:N46"/>
+    <mergeCell ref="O43:S46"/>
+    <mergeCell ref="T41:Y46"/>
+    <mergeCell ref="Z41:AZ42"/>
+    <mergeCell ref="Z43:AH43"/>
+    <mergeCell ref="AI43:AQ43"/>
+    <mergeCell ref="AR43:AZ43"/>
+    <mergeCell ref="Z44:AC46"/>
+    <mergeCell ref="AD44:AH46"/>
+    <mergeCell ref="AI44:AL46"/>
+    <mergeCell ref="AM44:AQ46"/>
+    <mergeCell ref="AR44:AU46"/>
+    <mergeCell ref="AV44:AZ46"/>
+    <mergeCell ref="BA41:BQ46"/>
+    <mergeCell ref="BR41:BX46"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="E47:N47"/>
+    <mergeCell ref="O47:S47"/>
+    <mergeCell ref="T47:Y47"/>
+    <mergeCell ref="Z47:AC47"/>
+    <mergeCell ref="AD47:AH47"/>
+    <mergeCell ref="AI47:AL47"/>
+    <mergeCell ref="AM47:AQ47"/>
+    <mergeCell ref="AR47:AU47"/>
+    <mergeCell ref="AV47:AZ47"/>
+    <mergeCell ref="BA47:BQ47"/>
+    <mergeCell ref="BR47:BX47"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="E48:N48"/>
+    <mergeCell ref="O48:S48"/>
+    <mergeCell ref="T48:Y48"/>
+    <mergeCell ref="Z48:AC48"/>
+    <mergeCell ref="AD48:AH48"/>
+    <mergeCell ref="AI48:AL48"/>
+    <mergeCell ref="AM48:AQ48"/>
+    <mergeCell ref="AR48:AU48"/>
+    <mergeCell ref="AV48:AZ48"/>
+    <mergeCell ref="BA48:BQ48"/>
+    <mergeCell ref="BR48:BX48"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="E49:N49"/>
+    <mergeCell ref="O49:S49"/>
+    <mergeCell ref="T49:Y49"/>
+    <mergeCell ref="Z49:AC49"/>
+    <mergeCell ref="AD49:AH49"/>
+    <mergeCell ref="AI49:AL49"/>
+    <mergeCell ref="AM49:AQ49"/>
+    <mergeCell ref="AR49:AU49"/>
+    <mergeCell ref="AV49:AZ49"/>
+    <mergeCell ref="BA49:BQ49"/>
+    <mergeCell ref="BR49:BX49"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="E50:N50"/>
+    <mergeCell ref="O50:S50"/>
+    <mergeCell ref="T50:Y50"/>
+    <mergeCell ref="Z50:AC50"/>
+    <mergeCell ref="AD50:AH50"/>
+    <mergeCell ref="AI50:AL50"/>
+    <mergeCell ref="AM50:AQ50"/>
+    <mergeCell ref="AR50:AU50"/>
+    <mergeCell ref="AV50:AZ50"/>
+    <mergeCell ref="BA50:BQ50"/>
+    <mergeCell ref="BR50:BX50"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="E51:N51"/>
+    <mergeCell ref="O51:S51"/>
+    <mergeCell ref="T51:Y51"/>
+    <mergeCell ref="Z51:AC51"/>
+    <mergeCell ref="AD51:AH51"/>
+    <mergeCell ref="AI51:AL51"/>
+    <mergeCell ref="AM51:AQ51"/>
+    <mergeCell ref="AR51:AU51"/>
+    <mergeCell ref="AV51:AZ51"/>
+    <mergeCell ref="BA51:BQ51"/>
+    <mergeCell ref="BR51:BX51"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="E52:N52"/>
+    <mergeCell ref="O52:S52"/>
+    <mergeCell ref="T52:Y52"/>
+    <mergeCell ref="Z52:AC52"/>
+    <mergeCell ref="AD52:AH52"/>
+    <mergeCell ref="AI52:AL52"/>
+    <mergeCell ref="AM52:AQ52"/>
+    <mergeCell ref="AR52:AU52"/>
+    <mergeCell ref="AV52:AZ52"/>
+    <mergeCell ref="BA52:BQ52"/>
+    <mergeCell ref="BR52:BX52"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="E53:N53"/>
+    <mergeCell ref="O53:S53"/>
+    <mergeCell ref="T53:Y53"/>
+    <mergeCell ref="Z53:AC53"/>
+    <mergeCell ref="AD53:AH53"/>
+    <mergeCell ref="AI53:AL53"/>
+    <mergeCell ref="AM53:AQ53"/>
+    <mergeCell ref="AR53:AU53"/>
+    <mergeCell ref="AV53:AZ53"/>
+    <mergeCell ref="BA53:BQ53"/>
+    <mergeCell ref="BR53:BX53"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="E54:N54"/>
+    <mergeCell ref="O54:S54"/>
+    <mergeCell ref="T54:Y54"/>
+    <mergeCell ref="Z54:AC54"/>
+    <mergeCell ref="AD54:AH54"/>
+    <mergeCell ref="AI54:AL54"/>
+    <mergeCell ref="AM54:AQ54"/>
+    <mergeCell ref="AR54:AU54"/>
+    <mergeCell ref="AV54:AZ54"/>
+    <mergeCell ref="BA54:BQ54"/>
+    <mergeCell ref="BR54:BX54"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="E55:N55"/>
+    <mergeCell ref="O55:S55"/>
+    <mergeCell ref="T55:Y55"/>
+    <mergeCell ref="Z55:AC55"/>
+    <mergeCell ref="AD55:AH55"/>
+    <mergeCell ref="AI55:AL55"/>
+    <mergeCell ref="AM55:AQ55"/>
+    <mergeCell ref="AR55:AU55"/>
+    <mergeCell ref="AV55:AZ55"/>
+    <mergeCell ref="BA55:BQ55"/>
+    <mergeCell ref="BR55:BX55"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="E56:N56"/>
+    <mergeCell ref="O56:S56"/>
+    <mergeCell ref="T56:Y56"/>
+    <mergeCell ref="Z56:AC56"/>
+    <mergeCell ref="AD56:AH56"/>
+    <mergeCell ref="AI56:AL56"/>
+    <mergeCell ref="AM56:AQ56"/>
+    <mergeCell ref="AR56:AU56"/>
+    <mergeCell ref="AV56:AZ56"/>
+    <mergeCell ref="BA56:BQ56"/>
+    <mergeCell ref="BR56:BX56"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="E57:N57"/>
+    <mergeCell ref="O57:S57"/>
+    <mergeCell ref="T57:Y57"/>
+    <mergeCell ref="Z57:AC57"/>
+    <mergeCell ref="AD57:AH57"/>
+    <mergeCell ref="AI57:AL57"/>
+    <mergeCell ref="AM57:AQ57"/>
+    <mergeCell ref="AR57:AU57"/>
+    <mergeCell ref="AV57:AZ57"/>
+    <mergeCell ref="BA57:BQ57"/>
+    <mergeCell ref="BR57:BX57"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="E58:N58"/>
+    <mergeCell ref="O58:S58"/>
+    <mergeCell ref="T58:Y58"/>
+    <mergeCell ref="Z58:AC58"/>
+    <mergeCell ref="AD58:AH58"/>
+    <mergeCell ref="AI58:AL58"/>
+    <mergeCell ref="AM58:AQ58"/>
+    <mergeCell ref="AR58:AU58"/>
+    <mergeCell ref="AV58:AZ58"/>
+    <mergeCell ref="BA58:BQ58"/>
+    <mergeCell ref="BR58:BX58"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="E59:N59"/>
+    <mergeCell ref="O59:S59"/>
+    <mergeCell ref="T59:Y59"/>
+    <mergeCell ref="Z59:AC59"/>
+    <mergeCell ref="AD59:AH59"/>
+    <mergeCell ref="AI59:AL59"/>
+    <mergeCell ref="AM59:AQ59"/>
+    <mergeCell ref="AR59:AU59"/>
+    <mergeCell ref="AV59:AZ59"/>
+    <mergeCell ref="BA59:BQ59"/>
+    <mergeCell ref="BR59:BX59"/>
+    <mergeCell ref="AI60:BF60"/>
+    <mergeCell ref="AI61:BF61"/>
+    <mergeCell ref="N64:AB64"/>
+    <mergeCell ref="AD64:AO64"/>
+    <mergeCell ref="AQ64:BO64"/>
+    <mergeCell ref="N65:AB65"/>
+    <mergeCell ref="AD65:AO65"/>
+    <mergeCell ref="AQ65:BO65"/>
+    <mergeCell ref="N66:AB66"/>
+    <mergeCell ref="AD66:AO66"/>
+    <mergeCell ref="AQ66:BO66"/>
+    <mergeCell ref="N67:AB67"/>
+    <mergeCell ref="AD67:AO67"/>
+    <mergeCell ref="AQ67:BO67"/>
+    <mergeCell ref="N68:AB68"/>
+    <mergeCell ref="AD68:AO68"/>
+    <mergeCell ref="AQ68:BO68"/>
+    <mergeCell ref="N69:AB69"/>
+    <mergeCell ref="AD69:AO69"/>
+    <mergeCell ref="AQ69:BO69"/>
+    <mergeCell ref="N70:AB70"/>
+    <mergeCell ref="AD70:AO70"/>
+    <mergeCell ref="AQ70:BO70"/>
+    <mergeCell ref="N71:AB71"/>
+    <mergeCell ref="AD71:AO71"/>
+    <mergeCell ref="AQ71:BO71"/>
+    <mergeCell ref="N72:AB72"/>
+    <mergeCell ref="AD72:AO72"/>
+    <mergeCell ref="AQ72:BO72"/>
+    <mergeCell ref="N73:AB73"/>
+    <mergeCell ref="AD73:AO73"/>
+    <mergeCell ref="AQ73:BO73"/>
+    <mergeCell ref="N74:AB74"/>
+    <mergeCell ref="AD74:AO74"/>
+    <mergeCell ref="AQ74:BO74"/>
+    <mergeCell ref="N75:AB75"/>
+    <mergeCell ref="AD75:AO75"/>
+    <mergeCell ref="AQ75:BO75"/>
+    <mergeCell ref="A78:BX82"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>